<commit_message>
Refactor: método 'build_excel_sheet' movido para a classe 'InterventorDAO' como método estático.
</commit_message>
<xml_diff>
--- a/src/data/excel_sheets_fca/to_send/2022-06-17_noticias_candidatas_para_ACF.xlsx
+++ b/src/data/excel_sheets_fca/to_send/2022-06-17_noticias_candidatas_para_ACF.xlsx
@@ -116,10 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,75 +450,75 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="250.7109375" customWidth="1"/>
+    <col min="2" max="2" width="125.7109375" style="2" customWidth="1"/>
     <col min="3" max="4" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="35" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="35" customHeight="1">
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="35" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="35" customHeight="1">
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="35" customHeight="1">
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>